<commit_message>
Matura 2015 Zadanie 4
Zadanie 4 ostateczna wersja :)
</commit_message>
<xml_diff>
--- a/Matura2015.xlsx
+++ b/Matura2015.xlsx
@@ -4,18 +4,24 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="4.2" sheetId="1" r:id="rId1"/>
-    <sheet name="Dane" sheetId="2" r:id="rId2"/>
+    <sheet name="4.4" sheetId="3" r:id="rId2"/>
+    <sheet name="4.5" sheetId="4" r:id="rId3"/>
+    <sheet name="4.3" sheetId="5" r:id="rId4"/>
+    <sheet name="Dane" sheetId="2" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="102">
   <si>
     <t>Kwartał</t>
   </si>
@@ -327,7 +333,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +348,28 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1E2832"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008CBA"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -362,10 +390,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,8 +402,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -388,6 +421,179 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="2"/>
+      <sheetName val="3"/>
+      <sheetName val="4"/>
+      <sheetName val="5"/>
+      <sheetName val="Wykres1"/>
+      <sheetName val="Dane"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="44">
+          <cell r="C44" t="str">
+            <v>Dama</v>
+          </cell>
+          <cell r="D44" t="str">
+            <v>Granta</v>
+          </cell>
+          <cell r="E44" t="str">
+            <v>Dorkas</v>
+          </cell>
+          <cell r="F44" t="str">
+            <v>Lodera</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="B45">
+            <v>2005</v>
+          </cell>
+          <cell r="C45">
+            <v>972</v>
+          </cell>
+          <cell r="D45">
+            <v>822</v>
+          </cell>
+          <cell r="E45">
+            <v>864</v>
+          </cell>
+          <cell r="F45">
+            <v>1284</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="B46">
+            <v>2006</v>
+          </cell>
+          <cell r="C46">
+            <v>1042</v>
+          </cell>
+          <cell r="D46">
+            <v>905</v>
+          </cell>
+          <cell r="E46">
+            <v>963</v>
+          </cell>
+          <cell r="F46">
+            <v>1380</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="B47">
+            <v>2007</v>
+          </cell>
+          <cell r="C47">
+            <v>1122</v>
+          </cell>
+          <cell r="D47">
+            <v>1000</v>
+          </cell>
+          <cell r="E47">
+            <v>1075</v>
+          </cell>
+          <cell r="F47">
+            <v>1486</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="B48">
+            <v>2008</v>
+          </cell>
+          <cell r="C48">
+            <v>1203</v>
+          </cell>
+          <cell r="D48">
+            <v>1102</v>
+          </cell>
+          <cell r="E48">
+            <v>1201</v>
+          </cell>
+          <cell r="F48">
+            <v>1599</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="B49">
+            <v>2009</v>
+          </cell>
+          <cell r="C49">
+            <v>1296</v>
+          </cell>
+          <cell r="D49">
+            <v>1217</v>
+          </cell>
+          <cell r="E49">
+            <v>1343</v>
+          </cell>
+          <cell r="F49">
+            <v>1724</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="B50">
+            <v>2010</v>
+          </cell>
+          <cell r="C50">
+            <v>1332</v>
+          </cell>
+          <cell r="D50">
+            <v>1264</v>
+          </cell>
+          <cell r="E50">
+            <v>1400</v>
+          </cell>
+          <cell r="F50">
+            <v>1772</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="B51">
+            <v>2011</v>
+          </cell>
+          <cell r="C51">
+            <v>1292</v>
+          </cell>
+          <cell r="D51">
+            <v>1224</v>
+          </cell>
+          <cell r="E51">
+            <v>1330</v>
+          </cell>
+          <cell r="F51">
+            <v>1658</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="B52">
+            <v>2012</v>
+          </cell>
+          <cell r="C52">
+            <v>1228</v>
+          </cell>
+          <cell r="D52">
+            <v>1160</v>
+          </cell>
+          <cell r="E52">
+            <v>1224</v>
+          </cell>
+          <cell r="F52">
+            <v>1492</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -679,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2742,10 +2948,730 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>237</v>
+      </c>
+      <c r="C2" s="2">
+        <v>198</v>
+      </c>
+      <c r="D2" s="2">
+        <v>207</v>
+      </c>
+      <c r="E2" s="2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <f>ROUNDDOWN(102%*B2,0)</f>
+        <v>241</v>
+      </c>
+      <c r="C3" s="2">
+        <f>ROUNDDOWN(102.7%*C2,0)</f>
+        <v>203</v>
+      </c>
+      <c r="D3" s="2">
+        <f>ROUNDDOWN(103%*D2,0)</f>
+        <v>213</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E21" si="0">ROUNDDOWN(102%*E2,0)</f>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B21" si="1">ROUNDDOWN(102%*B3,0)</f>
+        <v>245</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C21" si="2">ROUNDDOWN(102.7%*C3,0)</f>
+        <v>208</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D21" si="3">ROUNDDOWN(103%*D3,0)</f>
+        <v>219</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="1"/>
+        <v>249</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="2"/>
+        <v>213</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="1"/>
+        <v>253</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="2"/>
+        <v>218</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="1"/>
+        <v>258</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="2"/>
+        <v>223</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="3"/>
+        <v>237</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>342</v>
+      </c>
+      <c r="H7">
+        <v>6967</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="1"/>
+        <v>263</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="2"/>
+        <v>229</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="3"/>
+        <v>244</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+      <c r="H8">
+        <v>9245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="1"/>
+        <v>268</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="2"/>
+        <v>235</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="3"/>
+        <v>251</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>354</v>
+      </c>
+      <c r="H9">
+        <v>6310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="1"/>
+        <v>273</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="2"/>
+        <v>241</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="3"/>
+        <v>258</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>361</v>
+      </c>
+      <c r="H10">
+        <v>6846</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="1"/>
+        <v>278</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="2"/>
+        <v>247</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="3"/>
+        <v>265</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" si="1"/>
+        <v>283</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="2"/>
+        <v>253</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="3"/>
+        <v>272</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="1"/>
+        <v>288</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="2"/>
+        <v>259</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="3"/>
+        <v>280</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>382</v>
+      </c>
+      <c r="H13">
+        <f>SUM(H7:H10)</f>
+        <v>29368</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="1"/>
+        <v>293</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="2"/>
+        <v>265</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="3"/>
+        <v>288</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="1"/>
+        <v>298</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="2"/>
+        <v>272</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="3"/>
+        <v>296</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>396</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" si="1"/>
+        <v>303</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="2"/>
+        <v>279</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="3"/>
+        <v>304</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>403</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" si="1"/>
+        <v>309</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="2"/>
+        <v>286</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="3"/>
+        <v>313</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>411</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="1"/>
+        <v>315</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="2"/>
+        <v>293</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="3"/>
+        <v>322</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="1"/>
+        <v>321</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="3"/>
+        <v>331</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" si="1"/>
+        <v>327</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="2"/>
+        <v>308</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="3"/>
+        <v>340</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="1"/>
+        <v>333</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="2"/>
+        <v>316</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="3"/>
+        <v>350</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="2">
+        <f>B21</f>
+        <v>333</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" ref="C22:E25" si="4">C21</f>
+        <v>316</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" ref="B23:B25" si="5">B22</f>
+        <v>333</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="4"/>
+        <v>316</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="5"/>
+        <v>333</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="4"/>
+        <v>316</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="5"/>
+        <v>333</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="4"/>
+        <v>316</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2">
+        <f>ROUNDDOWN(99%*B25,0)</f>
+        <v>329</v>
+      </c>
+      <c r="C26" s="2">
+        <f>ROUNDDOWN(98.8%*C25,0)</f>
+        <v>312</v>
+      </c>
+      <c r="D26" s="2">
+        <f>ROUNDDOWN(98.1%*D25,0)</f>
+        <v>343</v>
+      </c>
+      <c r="E26" s="2">
+        <f>ROUNDDOWN(97.5%*E25,0)</f>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" ref="B27:B33" si="6">ROUNDDOWN(99%*B26,0)</f>
+        <v>325</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" ref="C27:C33" si="7">ROUNDDOWN(98.8%*C26,0)</f>
+        <v>308</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" ref="D27:D33" si="8">ROUNDDOWN(98.1%*D26,0)</f>
+        <v>336</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" ref="E27:E33" si="9">ROUNDDOWN(97.5%*E26,0)</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="6"/>
+        <v>321</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="7"/>
+        <v>304</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="8"/>
+        <v>329</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="9"/>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="2">
+        <f t="shared" si="6"/>
+        <v>317</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="8"/>
+        <v>322</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="9"/>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2">
+        <f t="shared" si="6"/>
+        <v>313</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="7"/>
+        <v>296</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="8"/>
+        <v>315</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="9"/>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="2">
+        <f t="shared" si="6"/>
+        <v>309</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="7"/>
+        <v>292</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="8"/>
+        <v>309</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="9"/>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="2">
+        <f t="shared" si="6"/>
+        <v>305</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="7"/>
+        <v>288</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="8"/>
+        <v>303</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="9"/>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="2">
+        <f t="shared" si="6"/>
+        <v>301</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="7"/>
+        <v>284</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="8"/>
+        <v>297</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="9"/>
+        <v>358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3438,4 +4364,1423 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>237</v>
+      </c>
+      <c r="C2" s="2">
+        <v>198</v>
+      </c>
+      <c r="D2" s="2">
+        <v>207</v>
+      </c>
+      <c r="E2" s="2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <f>ROUNDDOWN(102%*B2,0)</f>
+        <v>241</v>
+      </c>
+      <c r="C3" s="2">
+        <f>ROUNDDOWN(102.7%*C2,0)</f>
+        <v>203</v>
+      </c>
+      <c r="D3" s="2">
+        <f>ROUNDDOWN(103%*D2,0)</f>
+        <v>213</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E21" si="0">ROUNDDOWN(102%*E2,0)</f>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B21" si="1">ROUNDDOWN(102%*B3,0)</f>
+        <v>245</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C21" si="2">ROUNDDOWN(102.7%*C3,0)</f>
+        <v>208</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D21" si="3">ROUNDDOWN(103%*D3,0)</f>
+        <v>219</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="1"/>
+        <v>249</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="2"/>
+        <v>213</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="1"/>
+        <v>253</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="2"/>
+        <v>218</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="1"/>
+        <v>258</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="2"/>
+        <v>223</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="3"/>
+        <v>237</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="1"/>
+        <v>263</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="2"/>
+        <v>229</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="3"/>
+        <v>244</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="1"/>
+        <v>268</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="2"/>
+        <v>235</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="3"/>
+        <v>251</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="1"/>
+        <v>273</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="2"/>
+        <v>241</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="3"/>
+        <v>258</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="1"/>
+        <v>278</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="2"/>
+        <v>247</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="3"/>
+        <v>265</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" si="1"/>
+        <v>283</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="2"/>
+        <v>253</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="3"/>
+        <v>272</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="1"/>
+        <v>288</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="2"/>
+        <v>259</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="3"/>
+        <v>280</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="1"/>
+        <v>293</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="2"/>
+        <v>265</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="3"/>
+        <v>288</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="1"/>
+        <v>298</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="2"/>
+        <v>272</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="3"/>
+        <v>296</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" si="1"/>
+        <v>303</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="2"/>
+        <v>279</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="3"/>
+        <v>304</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" si="1"/>
+        <v>309</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="2"/>
+        <v>286</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="3"/>
+        <v>313</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="1"/>
+        <v>315</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="2"/>
+        <v>293</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="3"/>
+        <v>322</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="1"/>
+        <v>321</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="3"/>
+        <v>331</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" si="1"/>
+        <v>327</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="2"/>
+        <v>308</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="3"/>
+        <v>340</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="1"/>
+        <v>333</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="2"/>
+        <v>316</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="3"/>
+        <v>350</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="2">
+        <f>B21</f>
+        <v>333</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" ref="C22:E25" si="4">C21</f>
+        <v>316</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" ref="B23:B25" si="5">B22</f>
+        <v>333</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="4"/>
+        <v>316</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="5"/>
+        <v>333</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="4"/>
+        <v>316</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="5"/>
+        <v>333</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="4"/>
+        <v>316</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2">
+        <f>ROUNDDOWN(99%*B25,0)</f>
+        <v>329</v>
+      </c>
+      <c r="C26" s="2">
+        <f>ROUNDDOWN(98.8%*C25,0)</f>
+        <v>312</v>
+      </c>
+      <c r="D26" s="2">
+        <f>ROUNDDOWN(98.1%*D25,0)</f>
+        <v>343</v>
+      </c>
+      <c r="E26" s="2">
+        <f>ROUNDDOWN(97.5%*E25,0)</f>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" ref="B27:B33" si="6">ROUNDDOWN(99%*B26,0)</f>
+        <v>325</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" ref="C27:C33" si="7">ROUNDDOWN(98.8%*C26,0)</f>
+        <v>308</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" ref="D27:D33" si="8">ROUNDDOWN(98.1%*D26,0)</f>
+        <v>336</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" ref="E27:E33" si="9">ROUNDDOWN(97.5%*E26,0)</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="6"/>
+        <v>321</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="7"/>
+        <v>304</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="8"/>
+        <v>329</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="9"/>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="2">
+        <f t="shared" si="6"/>
+        <v>317</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="8"/>
+        <v>322</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="9"/>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2">
+        <f t="shared" si="6"/>
+        <v>313</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="7"/>
+        <v>296</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="8"/>
+        <v>315</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="9"/>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="2">
+        <f t="shared" si="6"/>
+        <v>309</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="7"/>
+        <v>292</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="8"/>
+        <v>309</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="9"/>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="2">
+        <f t="shared" si="6"/>
+        <v>305</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="7"/>
+        <v>288</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="8"/>
+        <v>303</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="9"/>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="2">
+        <f t="shared" si="6"/>
+        <v>301</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="7"/>
+        <v>284</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="8"/>
+        <v>297</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="9"/>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2">
+        <f>COUNTIF(B2:B33,"&gt;300")</f>
+        <v>18</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" ref="C34:E34" si="10">COUNTIF(C2:C33,"&gt;300")</f>
+        <v>9</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="10"/>
+        <v>17</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="10"/>
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="A1:E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>237</v>
+      </c>
+      <c r="C2" s="2">
+        <v>198</v>
+      </c>
+      <c r="D2" s="2">
+        <v>207</v>
+      </c>
+      <c r="E2" s="2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <f>ROUNDDOWN(102%*B2,0)</f>
+        <v>241</v>
+      </c>
+      <c r="C3" s="2">
+        <f>ROUNDDOWN(102.7%*C2,0)</f>
+        <v>203</v>
+      </c>
+      <c r="D3" s="2">
+        <f>ROUNDDOWN(103%*D2,0)</f>
+        <v>213</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E21" si="0">ROUNDDOWN(102%*E2,0)</f>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B21" si="1">ROUNDDOWN(102%*B3,0)</f>
+        <v>245</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C21" si="2">ROUNDDOWN(102.7%*C3,0)</f>
+        <v>208</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D21" si="3">ROUNDDOWN(103%*D3,0)</f>
+        <v>219</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="1"/>
+        <v>249</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="2"/>
+        <v>213</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="1"/>
+        <v>253</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="2"/>
+        <v>218</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="1"/>
+        <v>258</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="2"/>
+        <v>223</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="3"/>
+        <v>237</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="1"/>
+        <v>263</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="2"/>
+        <v>229</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="3"/>
+        <v>244</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="1"/>
+        <v>268</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="2"/>
+        <v>235</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="3"/>
+        <v>251</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="1"/>
+        <v>273</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="2"/>
+        <v>241</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="3"/>
+        <v>258</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="1"/>
+        <v>278</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="2"/>
+        <v>247</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="3"/>
+        <v>265</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" si="1"/>
+        <v>283</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="2"/>
+        <v>253</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="3"/>
+        <v>272</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="1"/>
+        <v>288</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="2"/>
+        <v>259</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="3"/>
+        <v>280</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="1"/>
+        <v>293</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="2"/>
+        <v>265</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="3"/>
+        <v>288</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="1"/>
+        <v>298</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="2"/>
+        <v>272</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="3"/>
+        <v>296</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" si="1"/>
+        <v>303</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="2"/>
+        <v>279</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="3"/>
+        <v>304</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" si="1"/>
+        <v>309</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="2"/>
+        <v>286</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="3"/>
+        <v>313</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="1"/>
+        <v>315</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="2"/>
+        <v>293</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="3"/>
+        <v>322</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="1"/>
+        <v>321</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="3"/>
+        <v>331</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" si="1"/>
+        <v>327</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="2"/>
+        <v>308</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="3"/>
+        <v>340</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="1"/>
+        <v>333</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="2"/>
+        <v>316</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="3"/>
+        <v>350</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="2">
+        <f>B21</f>
+        <v>333</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" ref="C22:E25" si="4">C21</f>
+        <v>316</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" ref="B23:B25" si="5">B22</f>
+        <v>333</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="4"/>
+        <v>316</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="5"/>
+        <v>333</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="4"/>
+        <v>316</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="5"/>
+        <v>333</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="4"/>
+        <v>316</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="4"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2">
+        <f>ROUNDDOWN(99%*B25,0)</f>
+        <v>329</v>
+      </c>
+      <c r="C26" s="2">
+        <f>ROUNDDOWN(98.8%*C25,0)</f>
+        <v>312</v>
+      </c>
+      <c r="D26" s="2">
+        <f>ROUNDDOWN(98.1%*D25,0)</f>
+        <v>343</v>
+      </c>
+      <c r="E26" s="2">
+        <f>ROUNDDOWN(97.5%*E25,0)</f>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" ref="B27:B33" si="6">ROUNDDOWN(99%*B26,0)</f>
+        <v>325</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" ref="C27:C33" si="7">ROUNDDOWN(98.8%*C26,0)</f>
+        <v>308</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" ref="D27:D33" si="8">ROUNDDOWN(98.1%*D26,0)</f>
+        <v>336</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" ref="E27:E33" si="9">ROUNDDOWN(97.5%*E26,0)</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="6"/>
+        <v>321</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="7"/>
+        <v>304</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="8"/>
+        <v>329</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="9"/>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="2">
+        <f t="shared" si="6"/>
+        <v>317</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="8"/>
+        <v>322</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="9"/>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2">
+        <f t="shared" si="6"/>
+        <v>313</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="7"/>
+        <v>296</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="8"/>
+        <v>315</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="9"/>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="2">
+        <f t="shared" si="6"/>
+        <v>309</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="7"/>
+        <v>292</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="8"/>
+        <v>309</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="9"/>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="2">
+        <f t="shared" si="6"/>
+        <v>305</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="7"/>
+        <v>288</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="8"/>
+        <v>303</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="9"/>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="2">
+        <f t="shared" si="6"/>
+        <v>301</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="7"/>
+        <v>284</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="8"/>
+        <v>297</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="9"/>
+        <v>358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>